<commit_message>
use entire name column for rename
</commit_message>
<xml_diff>
--- a/tools/prep/test-data/rename_with_column.xlsx
+++ b/tools/prep/test-data/rename_with_column.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">New Name</t>
   </si>
@@ -47,6 +47,15 @@
   </si>
   <si>
     <t xml:space="preserve">P22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spaced Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_047766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECA2</t>
   </si>
 </sst>
 </file>
@@ -56,11 +65,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -82,12 +92,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFC9211E"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -132,8 +137,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -141,7 +150,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -154,66 +163,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FFC9211E"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -225,46 +174,54 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2"/>
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
add _ for column
</commit_message>
<xml_diff>
--- a/tools/prep/test-data/rename_with_column.xlsx
+++ b/tools/prep/test-data/rename_with_column.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t xml:space="preserve">New Name</t>
+    <t xml:space="preserve">New_Name</t>
   </si>
   <si>
     <t xml:space="preserve">Acc</t>
@@ -174,10 +174,10 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -213,13 +213,13 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>